<commit_message>
Increase the size of the chart
</commit_message>
<xml_diff>
--- a/milestones/Gantt Chart.xlsx
+++ b/milestones/Gantt Chart.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,206 +77,22 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>StartDate</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Research</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Programing</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Statistic</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Writing</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>41685.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41690.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41699.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41705.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Duration</c:v>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Research</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Programing</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Statistic</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Writing</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="-2130040808"/>
-        <c:axId val="-2130039016"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-2130040808"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130039016"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2130039016"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="t"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130040808"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -305,6 +121,7 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -331,19 +148,19 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$5</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>d\-mmm</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>41685.0</c:v>
+                  <c:v>41685</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41690.0</c:v>
+                  <c:v>41690</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41699.0</c:v>
+                  <c:v>41699</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41705.0</c:v>
+                  <c:v>41705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -380,16 +197,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -405,11 +222,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2127035192"/>
-        <c:axId val="-2124236760"/>
+        <c:axId val="169077376"/>
+        <c:axId val="170594688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127035192"/>
+        <c:axId val="169077376"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -418,7 +235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124236760"/>
+        <c:crossAx val="170594688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -426,35 +243,30 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124236760"/>
+        <c:axId val="170594688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="41685.0"/>
+          <c:min val="41685"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127035192"/>
+        <c:crossAx val="169077376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -464,46 +276,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215899</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -516,7 +298,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -850,12 +632,12 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -866,7 +648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -877,7 +659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -888,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -899,7 +681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -912,7 +694,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Cleaned up word doc, made a Gantt chart, and added steps to put Ant into Eclipse
</commit_message>
<xml_diff>
--- a/milestones/Gantt Chart.xlsx
+++ b/milestones/Gantt Chart.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Detailed Gantt Chart and Plan" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,34 +19,136 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>Writing</t>
-  </si>
-  <si>
-    <t>Programing</t>
-  </si>
-  <si>
-    <t>Statistic</t>
-  </si>
-  <si>
-    <t>Work</t>
-  </si>
-  <si>
-    <t>StartDate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>PLANNED</t>
+  </si>
+  <si>
+    <t>ACTUAL</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Duration (Days)</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Research Topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research </t>
+  </si>
+  <si>
+    <t>DB Design (to store SVN log data)</t>
+  </si>
+  <si>
+    <t>SVN Log parse, extract, import</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Learn about Eclipse Plugins</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Implement simple metric</t>
+  </si>
+  <si>
+    <t>Implement complex metrics</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Test data creation</t>
+  </si>
+  <si>
+    <t>Test code implementation</t>
+  </si>
+  <si>
+    <t>Regression testing</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Collect data for Ant (Measure)</t>
+  </si>
+  <si>
+    <t>Analyze Metrics</t>
+  </si>
+  <si>
+    <t>Final Report</t>
+  </si>
+  <si>
+    <t>Report - Introduction</t>
+  </si>
+  <si>
+    <t>Report - Previous work</t>
+  </si>
+  <si>
+    <t>Report - Results (statistics)</t>
+  </si>
+  <si>
+    <t>Report - Analysis</t>
+  </si>
+  <si>
+    <t>Report - Conclusion and abstract</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>SA, VR</t>
+  </si>
+  <si>
+    <t>SA, TR</t>
+  </si>
+  <si>
+    <t>TR, AG</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>VR, AG</t>
+  </si>
+  <si>
+    <t>AG, VR</t>
+  </si>
+  <si>
+    <t>SA, AG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,16 +156,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -71,16 +208,489 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -99,10 +709,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -116,51 +726,131 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Start Date</c:v>
+          </c:tx>
           <c:spPr>
             <a:noFill/>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>'Detailed Gantt Chart and Plan'!$D$4:$D$20</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>Research</c:v>
+                  <c:v>Research </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Programing</c:v>
+                  <c:v>DB Design (to store SVN log data)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Statistic</c:v>
+                  <c:v>SVN Log parse, extract, import</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Writing</c:v>
+                  <c:v>Learn about Eclipse Plugins</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Design</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Implement simple metric</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Implement complex metrics</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Test data creation</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Test code implementation</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Regression testing</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Collect data for Ant (Measure)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Analyze Metrics</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Report - Introduction</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Report - Previous work</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Report - Results (statistics)</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Report - Analysis</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Report - Conclusion and abstract</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>'Detailed Gantt Chart and Plan'!$E$4:$E$20</c:f>
               <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>41685</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41690</c:v>
+                  <c:v>41680</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>41686</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41688</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41697</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>41699</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>41705</c:v>
+                <c:pt idx="6">
+                  <c:v>41708</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41708</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41718</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41706</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41713</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41721</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41733</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41740</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -169,44 +859,125 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Duration</c:v>
+          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>'Detailed Gantt Chart and Plan'!$D$4:$D$20</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>Research</c:v>
+                  <c:v>Research </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Programing</c:v>
+                  <c:v>DB Design (to store SVN log data)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Statistic</c:v>
+                  <c:v>SVN Log parse, extract, import</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Writing</c:v>
+                  <c:v>Learn about Eclipse Plugins</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Design</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Implement simple metric</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Implement complex metrics</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Test data creation</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Test code implementation</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Regression testing</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Collect data for Ant (Measure)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Analyze Metrics</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Report - Introduction</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Report - Previous work</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Report - Results (statistics)</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Report - Analysis</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Report - Conclusion and abstract</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:f>'Detailed Gantt Chart and Plan'!$F$4:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -222,11 +993,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="169077376"/>
-        <c:axId val="170594688"/>
+        <c:axId val="68092672"/>
+        <c:axId val="48943872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169077376"/>
+        <c:axId val="68092672"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -235,7 +1006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170594688"/>
+        <c:crossAx val="48943872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -243,7 +1014,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170594688"/>
+        <c:axId val="48943872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41685"/>
@@ -251,13 +1022,14 @@
         <c:delete val="0"/>
         <c:axPos val="t"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169077376"/>
+        <c:crossAx val="68092672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="14"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -266,7 +1038,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -277,20 +1049,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>215899</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>174625</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -629,77 +1403,477 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="B2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="1.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="37" customWidth="1"/>
+    <col min="6" max="6" width="13" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.25" style="37" customWidth="1"/>
+    <col min="9" max="11" width="15" style="37" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
+      <c r="E2" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="47"/>
+      <c r="K2" s="48"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H3" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="K3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7">
         <v>41685</v>
       </c>
-      <c r="C2">
+      <c r="F4" s="8">
+        <v>40</v>
+      </c>
+      <c r="G4" s="9">
+        <f>E4+F4</f>
+        <v>41725</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="45"/>
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="13">
+        <v>41680</v>
+      </c>
+      <c r="F5" s="14">
+        <v>14</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="45"/>
+      <c r="D6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="19">
+        <v>41686</v>
+      </c>
+      <c r="F6" s="20">
+        <v>10</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="7">
+        <v>41688</v>
+      </c>
+      <c r="F7" s="8">
+        <v>12</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" ref="G7:G20" si="0">E7+F7</f>
+        <v>41700</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="45"/>
+      <c r="D8" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>41690</v>
-      </c>
-      <c r="C3">
+      <c r="E8" s="13">
+        <v>41697</v>
+      </c>
+      <c r="F8" s="14">
+        <v>5</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="45"/>
+      <c r="D9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="13">
+        <v>41699</v>
+      </c>
+      <c r="F9" s="14">
+        <v>10</v>
+      </c>
+      <c r="G9" s="15">
+        <f t="shared" si="0"/>
+        <v>41709</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="45"/>
+      <c r="D10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="19">
+        <v>41708</v>
+      </c>
+      <c r="F10" s="20">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>41699</v>
-      </c>
-      <c r="C4">
+      <c r="G10" s="21">
+        <f t="shared" si="0"/>
+        <v>41723</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="25">
+        <v>41700</v>
+      </c>
+      <c r="F11" s="26">
+        <v>15</v>
+      </c>
+      <c r="G11" s="27">
+        <f>E11+F11</f>
+        <v>41715</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="45"/>
+      <c r="D12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="13">
+        <v>41702</v>
+      </c>
+      <c r="F12" s="14">
+        <v>15</v>
+      </c>
+      <c r="G12" s="15">
+        <f>E12+F12</f>
+        <v>41717</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="45"/>
+      <c r="D13" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="31">
+        <v>41708</v>
+      </c>
+      <c r="F13" s="32">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41705</v>
-      </c>
-      <c r="C5">
+      <c r="G13" s="33">
+        <f>E13+F13</f>
+        <v>41718</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="7">
+        <v>41718</v>
+      </c>
+      <c r="F14" s="8">
+        <v>5</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>41723</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="45"/>
+      <c r="D15" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="19">
+        <v>41721</v>
+      </c>
+      <c r="F15" s="20">
         <v>10</v>
       </c>
+      <c r="G15" s="21">
+        <f t="shared" si="0"/>
+        <v>41731</v>
+      </c>
+      <c r="H15" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="25">
+        <v>41706</v>
+      </c>
+      <c r="F16" s="26">
+        <v>7</v>
+      </c>
+      <c r="G16" s="27">
+        <f t="shared" si="0"/>
+        <v>41713</v>
+      </c>
+      <c r="H16" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="28"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="45"/>
+      <c r="D17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="13">
+        <v>41713</v>
+      </c>
+      <c r="F17" s="14">
+        <v>10</v>
+      </c>
+      <c r="G17" s="15">
+        <f t="shared" si="0"/>
+        <v>41723</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="45"/>
+      <c r="D18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="13">
+        <v>41721</v>
+      </c>
+      <c r="F18" s="14">
+        <v>15</v>
+      </c>
+      <c r="G18" s="15">
+        <f t="shared" si="0"/>
+        <v>41736</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="45"/>
+      <c r="D19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="13">
+        <v>41733</v>
+      </c>
+      <c r="F19" s="14">
+        <v>8</v>
+      </c>
+      <c r="G19" s="15">
+        <f t="shared" si="0"/>
+        <v>41741</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="17"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="45"/>
+      <c r="D20" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="19">
+        <v>41740</v>
+      </c>
+      <c r="F20" s="20">
+        <v>5</v>
+      </c>
+      <c r="G20" s="21">
+        <f t="shared" si="0"/>
+        <v>41745</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="22"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+    </row>
+    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+    </row>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <mergeCells count="7">
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>